<commit_message>
Integrated lab test plotting and excel interface integrated PSD plotting
</commit_message>
<xml_diff>
--- a/Input_files/Python_CPT_Input_Template.xlsx
+++ b/Input_files/Python_CPT_Input_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sc\PycharmProjects\cpt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sc\PycharmProjects\SI_processing_automation\Input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14748" windowHeight="5268"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="14745" windowHeight="5265"/>
   </bookViews>
   <sheets>
     <sheet name="Global_variable" sheetId="3" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>plot_list</t>
   </si>
@@ -134,9 +134,6 @@
     <t>Plot CPT</t>
   </si>
   <si>
-    <t>C:\Users\sc\PycharmProjects\cpt\Hornsea-Two</t>
-  </si>
-  <si>
     <t>SCPT file name</t>
   </si>
   <si>
@@ -185,15 +182,6 @@
     <t>.png</t>
   </si>
   <si>
-    <t>C:\Users\sc\PycharmProjects\cpt</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\cpt\RWE-Taiwan</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\cpt\CPT-fig\RWE-Taiwan</t>
-  </si>
-  <si>
     <t>SCPT-combined.xlsx</t>
   </si>
   <si>
@@ -213,6 +201,21 @@
   </si>
   <si>
     <t>BH09-TAICHUNG</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Input_files\cpt_data_files\RWE-Taiwan</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Input_files\ags-db</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\Processed-CPT</t>
   </si>
 </sst>
 </file>
@@ -575,18 +578,18 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -594,77 +597,77 @@
         <v>10</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="b">
         <v>0</v>
@@ -676,9 +679,9 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="b">
         <v>1</v>
@@ -690,7 +693,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -698,7 +701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -706,95 +709,95 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="C20" t="s">
         <v>26</v>
       </c>
-      <c r="C20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D24" s="8"/>
     </row>
@@ -814,12 +817,12 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -838,13 +841,13 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
AMB: 1. figure_class: Reduced the spaced between subplots 2. main: Change the axis labels to have subscripts 3. main: Change to get the stratigraphy colors from input excel file
</commit_message>
<xml_diff>
--- a/Input_files/Python_CPT_Input_Template.xlsx
+++ b/Input_files/Python_CPT_Input_Template.xlsx
@@ -1,37 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sc\PycharmProjects\SI_processing_automation\Input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amb\PycharmProjects\SI_processing_automation\Input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6879BA-AB16-49C5-B810-B2329016A89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="14745" windowHeight="5265"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global_variable" sheetId="3" r:id="rId1"/>
-    <sheet name="Single_plot_input" sheetId="1" r:id="rId2"/>
-    <sheet name="Side_by_side_plot_input" sheetId="2" r:id="rId3"/>
+    <sheet name="stratigraphy_color_dict" sheetId="4" r:id="rId2"/>
+    <sheet name="Single_plot_input" sheetId="1" r:id="rId3"/>
+    <sheet name="Side_by_side_plot_input" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Serena Che</author>
   </authors>
   <commentList>
-    <comment ref="B24" authorId="0" shapeId="0">
+    <comment ref="B24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -55,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C24" authorId="0" shapeId="0">
+    <comment ref="C24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>plot_list</t>
   </si>
@@ -179,15 +191,9 @@
     <t>Figure_extension</t>
   </si>
   <si>
-    <t>.png</t>
-  </si>
-  <si>
     <t>SCPT-combined.xlsx</t>
   </si>
   <si>
-    <t>gcg - new.gpj</t>
-  </si>
-  <si>
     <t>SCPG-combined.xlsx</t>
   </si>
   <si>
@@ -197,31 +203,61 @@
     <t>SOIL_PROPERTY-combined.xlsx</t>
   </si>
   <si>
-    <t>BH06-TAICHUNG</t>
-  </si>
-  <si>
-    <t>BH09-TAICHUNG</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Input_files\cpt_data_files\RWE-Taiwan</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Input_files\ags-db</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\Processed-CPT</t>
+    <t>.svg</t>
+  </si>
+  <si>
+    <t>C:\Users\amb\PycharmProjects\SI_processing_automation</t>
+  </si>
+  <si>
+    <t>S:\Clients\T-Z\Thor Wind Farm\02_Working\CPT-data\EOS\EOS-BH-01\CPT-fig</t>
+  </si>
+  <si>
+    <t>S:\Clients\T-Z\Thor Wind Farm\02_Working\CPT-data\EOS\EOS-BH-01</t>
+  </si>
+  <si>
+    <t>Thor_Fugro-2022-SI.gpj</t>
+  </si>
+  <si>
+    <t>EOS-BH-01</t>
+  </si>
+  <si>
+    <t>S:\Clients\T-Z\Thor Wind Farm\02_Working\Gint_databases</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>U40-SAND</t>
+  </si>
+  <si>
+    <t>U46-CLAY</t>
+  </si>
+  <si>
+    <t>U98-CLAY</t>
+  </si>
+  <si>
+    <t>U98-SAND</t>
+  </si>
+  <si>
+    <t>#E0D68D</t>
+  </si>
+  <si>
+    <t>#228833</t>
+  </si>
+  <si>
+    <t>#802659</t>
+  </si>
+  <si>
+    <t>#F1D1E3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -573,12 +609,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +643,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1"/>
@@ -618,7 +654,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -629,11 +665,9 @@
         <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
@@ -642,7 +676,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -653,7 +687,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -670,7 +704,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="str">
         <f>IF(AND($B$8=TRUE,$B$9=TRUE),"Cannot be True at the same time","ok")</f>
@@ -684,7 +718,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="str">
         <f>IF(AND($B$8=TRUE,$B$9=TRUE),"Cannot be True at the same time","ok")</f>
@@ -714,7 +748,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -726,7 +760,7 @@
         <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
@@ -737,7 +771,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
@@ -748,7 +782,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
@@ -759,7 +793,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
         <v>24</v>
@@ -794,11 +828,9 @@
         <v>29</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>38</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
   </sheetData>
@@ -809,12 +841,70 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97D0C77-CF34-4830-A02F-345B9F600E1D}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,13 +922,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>